<commit_message>
json table 동작 확인
</commit_message>
<xml_diff>
--- a/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
+++ b/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IK-LPC-020\Documents\GitHub\REngine\Assets\bin\graphics\table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\menew\Documents\GitHub\REngine\Assets\bin\graphics\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{683804D8-20E3-4BCA-BB18-42C2F01AAEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A6524E-A8CD-415D-94F3-101D523FC297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
+    <workbookView xWindow="3075" yWindow="4935" windowWidth="25410" windowHeight="11385" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,74 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>../PipelineLayoutTable.json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UUID : String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count : Integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description : String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResourceType : String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BindFlags : Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StageFlags : Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slot : Integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ArraySize : Integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkyBox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Texture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sampler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WrapLinear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fe6f153f-d693-4675-9b0e-65b8be91f35b</t>
+  </si>
+  <si>
+    <t>"ShaderResource"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"PS"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -97,10 +165,27 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{354EB2B6-19B7-49DB-AC62-9278FDC0CB99}" name="표1" displayName="표1" ref="A2:H11" totalsRowShown="0">
+  <autoFilter ref="A2:H11" xr:uid="{354EB2B6-19B7-49DB-AC62-9278FDC0CB99}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{36A100E7-56AC-420F-A1E5-97EB4F3C0948}" name="UUID : String"/>
+    <tableColumn id="2" xr3:uid="{78A49022-DCE6-4CA9-A406-02645D160AEF}" name="Count : Integer"/>
+    <tableColumn id="3" xr3:uid="{F3FD9AE5-975D-42C0-81B3-CC0CD5CB68D3}" name="Description : String"/>
+    <tableColumn id="4" xr3:uid="{67021DE1-F4B2-446A-AC67-143EED20391B}" name="ResourceType : String"/>
+    <tableColumn id="5" xr3:uid="{5FE1C201-465F-4487-8E84-D1B5E6C29FE3}" name="BindFlags : Array"/>
+    <tableColumn id="6" xr3:uid="{3C570FF2-8267-413D-98F3-65103D5420B0}" name="StageFlags : Array"/>
+    <tableColumn id="7" xr3:uid="{99703446-1FBF-4B80-9973-8037C7747D08}" name="Slot : Integer"/>
+    <tableColumn id="8" xr3:uid="{30DA032F-829B-489F-A32A-BC68CA4CE3F7}" name="ArraySize : Integer"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,7 +223,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -244,7 +329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,7 +471,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -394,13 +479,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8BBF2-956F-48E9-BBE6-729EE7E2F5E2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
material property class 추가
파이프라인를 생성시 property 관련 데이터를 생성하도록 만들고

머티리얼에서 파이프라인를 설정하면 property 데이터로부터 MaterialProptryBlock를 설정

MaterialPropertyBlock를 바인드하면 Const Buffer를 업데이트 및 바인드하고 리소스 또한 바인드

기존 파이프라인레이아웃은 PerMaterial이 아닌 contant buffer와 샘플러와 같은 것들만 이용하도록 이용방법 수정함
</commit_message>
<xml_diff>
--- a/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
+++ b/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\menew\Documents\GitHub\REngine\Assets\bin\graphics\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E8E190-FBB1-4EE9-857D-46AFF6EF36BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA10612-F5B3-4CB1-815A-20417A1E4EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="25410" windowHeight="11385" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="25410" windowHeight="11385" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>../PipelineLayoutTable.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,10 +78,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Texture</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sampler</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -90,13 +86,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fe6f153f-d693-4675-9b0e-65b8be91f35b</t>
-  </si>
-  <si>
-    <t>"ShaderResource"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"PS"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,11 +101,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"PS"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PerDebug</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Standard</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -501,7 +490,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -545,19 +534,16 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -567,17 +553,26 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
       <c r="G4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -585,25 +580,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>1</v>

</xml_diff>

<commit_message>
light component 관련 추가
light component 추가 및 관련 에디터 작업

property 중 enum과 color과 상호작용이 가능한 ComboBox, ColorEdit Widget 추가

material property block이 texturebuffer가 아닌 texture 포인터를 캐싱하도록 변경 및 관련 함수 수정(texture buffer로 만들어 지지 않는 텍스처를 바인딩 하기 위해 추가 ex) deferred light pass material의 camera gbuffer texture)
</commit_message>
<xml_diff>
--- a/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
+++ b/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\menew\Documents\GitHub\REngine\Assets\bin\graphics\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA10612-F5B3-4CB1-815A-20417A1E4EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3521423A-07E0-496D-9B3A-7414AE410C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="25410" windowHeight="11385" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="25410" windowHeight="11385" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>../PipelineLayoutTable.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,6 +106,17 @@
   </si>
   <si>
     <t>Standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deferred Light</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WrapLinear</t>
+  </si>
+  <si>
+    <t>ShadowLinearBorder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -130,20 +141,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -152,8 +182,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -174,8 +207,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{354EB2B6-19B7-49DB-AC62-9278FDC0CB99}" name="표1" displayName="표1" ref="A2:H11" totalsRowShown="0">
-  <autoFilter ref="A2:H11" xr:uid="{354EB2B6-19B7-49DB-AC62-9278FDC0CB99}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{354EB2B6-19B7-49DB-AC62-9278FDC0CB99}" name="표1" displayName="표1" ref="A2:H14" totalsRowShown="0">
+  <autoFilter ref="A2:H14" xr:uid="{354EB2B6-19B7-49DB-AC62-9278FDC0CB99}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{36A100E7-56AC-420F-A1E5-97EB4F3C0948}" name="UUID : String"/>
     <tableColumn id="2" xr3:uid="{78A49022-DCE6-4CA9-A406-02645D160AEF}" name="Count : Integer"/>
@@ -487,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8BBF2-956F-48E9-BBE6-729EE7E2F5E2}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:H5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -601,6 +634,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ibl pass 작업 추가
일단 sky box texture에 따라 ibl 관련 텍스처를 생성 할 수 있는 render pass 추가

조도 맵에서 아직 헷갈리는 부분이 있음 HDR 관련
</commit_message>
<xml_diff>
--- a/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
+++ b/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\menew\Documents\GitHub\REngine\Assets\bin\graphics\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3521423A-07E0-496D-9B3A-7414AE410C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687822D9-971B-4B3D-AC33-94B91564F3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="25410" windowHeight="11385" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>../PipelineLayoutTable.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -117,6 +117,14 @@
   </si>
   <si>
     <t>ShadowLinearBorder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IBL_Irradiance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IBL_Radiance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -520,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8BBF2-956F-48E9-BBE6-729EE7E2F5E2}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -674,6 +682,52 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
paranomic skybox hdr image 추가 ObjectButton widget 변경
파라노믹 스카이 박스의 리소스로 hdr 이미지를 사용하여 스카이 박스 렌더링 테스트함

상수 버퍼의 값에 0이 잘못들어가서 출력 값이 0이되는 것이였음 원인은 파악했으나 수정은 아직 안함

에셋 패스에서 로드 에셋할때 uuid를 넣고있던 버그 수정 패스를 넣도록 수정함

오브젝트 버튼 위젯을 다른 위젯들과 마찬가지로 위젯데이타를 상속 받도록 변경함
</commit_message>
<xml_diff>
--- a/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
+++ b/Assets/bin/graphics/table/PipelineLayoutTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\menew\Documents\GitHub\REngine\Assets\bin\graphics\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687822D9-971B-4B3D-AC33-94B91564F3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628148F1-2858-4803-8D9F-252737A106B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
+    <workbookView xWindow="2460" yWindow="2460" windowWidth="25410" windowHeight="11385" xr2:uid="{A66BFFD3-44BC-431C-A43B-437626919F3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>../PipelineLayoutTable.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,10 +74,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SkyBox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sampler</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -126,6 +122,13 @@
   <si>
     <t>IBL_Radiance</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkyBox-Cubed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skybox-Panoramic</t>
   </si>
 </sst>
 </file>
@@ -528,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8BBF2-956F-48E9-BBE6-729EE7E2F5E2}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -572,19 +575,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -595,22 +598,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -621,19 +624,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -644,19 +647,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -667,13 +670,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -684,19 +687,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
         <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -707,24 +710,47 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
         <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
     </row>

</xml_diff>